<commit_message>
2003 add resolve all sheet , fix bugs
</commit_message>
<xml_diff>
--- a/src/test/resources/data.xlsx
+++ b/src/test/resources/data.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MySpace\DailyCode\Java\poidemo\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD3E04B-D536-47D5-8B50-8977EE6AB21D}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10A2BA99-DCD4-409A-8574-C2E323177835}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22944" windowHeight="7068" xr2:uid="{BAA7A24D-D08E-4DAA-A977-7C5D7CD148A7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22944" windowHeight="7068" activeTab="1" xr2:uid="{BAA7A24D-D08E-4DAA-A977-7C5D7CD148A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="单元表2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -283,14 +283,14 @@
     <xf numFmtId="185" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="186" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -608,7 +608,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A0207466-FAB2-4AE5-BD23-69FA7FFB606B}">
   <dimension ref="A1:M8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -621,20 +621,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -687,7 +687,7 @@
       <c r="C3">
         <v>90</v>
       </c>
-      <c r="D3" s="20">
+      <c r="D3" s="18">
         <v>70.665999999999997</v>
       </c>
       <c r="E3">
@@ -910,7 +910,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9885DF67-47F2-433C-9377-987993F0E23E}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
@@ -961,15 +961,15 @@
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="20"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="20"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>